<commit_message>
working ond startCheck() functionality
</commit_message>
<xml_diff>
--- a/inv__db.xlsx
+++ b/inv__db.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="14040" windowHeight="12240" tabRatio="500"/>
+    <workbookView windowWidth="26550" windowHeight="12600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -9007,10 +9007,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -9058,8 +9058,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9073,96 +9147,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9175,8 +9161,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9190,17 +9184,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9215,7 +9215,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9227,7 +9239,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9245,7 +9269,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9257,7 +9299,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9269,7 +9335,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9281,13 +9347,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9299,25 +9365,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9335,67 +9395,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9427,8 +9427,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9437,7 +9437,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9453,15 +9468,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9496,21 +9502,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -9521,140 +9512,149 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
@@ -10097,7 +10097,7 @@
   <dimension ref="A1:K1048573"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
@@ -10147,7 +10147,9 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="12"/>
@@ -10164,7 +10166,9 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -10183,7 +10187,9 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>

</xml_diff>